<commit_message>
Update attribution prompt formatting
</commit_message>
<xml_diff>
--- a/XYZ_12312025_01312026.xlsx
+++ b/XYZ_12312025_01312026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisthelen/Documents/_code/contribnote/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28CB922-7BC0-854A-8175-B42FE0E27E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078179A9-74EF-BA49-8F02-65E26DDBDA8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AttributionbyCountryMasterRisk" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>Portfolio long name</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Total Effect</t>
-  </si>
-  <si>
-    <t>Country</t>
   </si>
   <si>
     <t>United States</t>
@@ -714,11 +711,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="4" width="15" customWidth="1"/>
@@ -818,7 +817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -871,92 +870,92 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9">
-        <v>69.2</v>
+        <v>6.9</v>
       </c>
       <c r="C9">
-        <v>67.599999999999994</v>
+        <v>6.5</v>
       </c>
       <c r="D9">
-        <v>68.400000000000006</v>
+        <v>6.7</v>
       </c>
       <c r="E9">
-        <v>3.85</v>
+        <v>5.2</v>
       </c>
       <c r="F9">
-        <v>2.63</v>
+        <v>0.35</v>
       </c>
       <c r="G9">
-        <v>70.8</v>
+        <v>7.2</v>
       </c>
       <c r="H9">
-        <v>69.400000000000006</v>
+        <v>6.8</v>
       </c>
       <c r="I9">
-        <v>70.099999999999994</v>
+        <v>6.9</v>
       </c>
       <c r="J9">
-        <v>3.42</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K9">
-        <v>2.41</v>
+        <v>0.31</v>
       </c>
       <c r="L9">
-        <v>-1.7</v>
+        <v>-0.2</v>
       </c>
       <c r="M9">
-        <v>0.43</v>
+        <v>0.6</v>
       </c>
       <c r="N9">
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="O9">
-        <v>-0.06</v>
+        <v>-0.01</v>
       </c>
       <c r="P9">
-        <v>0.18</v>
+        <v>0.05</v>
       </c>
       <c r="Q9">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10">
-        <v>6.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C10">
-        <v>6.5</v>
+        <v>3.9</v>
       </c>
       <c r="D10">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>5.2</v>
+        <v>4.7</v>
       </c>
       <c r="F10">
-        <v>0.35</v>
+        <v>0.19</v>
       </c>
       <c r="G10">
-        <v>7.2</v>
+        <v>4.3</v>
       </c>
       <c r="H10">
-        <v>6.8</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I10">
-        <v>6.9</v>
+        <v>4.2</v>
       </c>
       <c r="J10">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K10">
-        <v>0.31</v>
+        <v>0.17</v>
       </c>
       <c r="L10">
         <v>-0.2</v>
@@ -965,213 +964,213 @@
         <v>0.6</v>
       </c>
       <c r="N10">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="O10">
         <v>-0.01</v>
       </c>
       <c r="P10">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="Q10">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
       <c r="B11">
-        <v>4.0999999999999996</v>
+        <v>3.2</v>
       </c>
       <c r="C11">
-        <v>3.9</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="E11">
-        <v>4.7</v>
+        <v>2.8</v>
       </c>
       <c r="F11">
-        <v>0.19</v>
+        <v>0.09</v>
       </c>
       <c r="G11">
-        <v>4.3</v>
+        <v>3.5</v>
       </c>
       <c r="H11">
-        <v>4.0999999999999996</v>
+        <v>3.3</v>
       </c>
       <c r="I11">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="J11">
-        <v>4.0999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="K11">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="L11">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="M11">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="N11">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="O11">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="Q11">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
       <c r="B12">
-        <v>3.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="D12">
-        <v>3.1</v>
+        <v>5.3</v>
       </c>
       <c r="E12">
-        <v>2.8</v>
+        <v>1.2</v>
       </c>
       <c r="F12">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="G12">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="H12">
-        <v>3.3</v>
+        <v>4.3</v>
       </c>
       <c r="I12">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="J12">
-        <v>2.5</v>
+        <v>0.9</v>
       </c>
       <c r="K12">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="L12">
-        <v>-0.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M12">
         <v>0.3</v>
       </c>
       <c r="N12">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="P12">
         <v>0.01</v>
       </c>
       <c r="Q12">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13">
-        <v>5.0999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C13">
-        <v>5.5</v>
+        <v>1.2</v>
       </c>
       <c r="D13">
-        <v>5.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E13">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="F13">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="G13">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="H13">
-        <v>4.3</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>4.2</v>
+        <v>0.9</v>
       </c>
       <c r="J13">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="K13">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="L13">
-        <v>1.1000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="M13">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="N13">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="O13">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0.01</v>
       </c>
       <c r="Q13">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
       <c r="B14">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0.9</v>
+      </c>
+      <c r="E14">
+        <v>1.6</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14">
+        <v>0.8</v>
+      </c>
+      <c r="H14">
+        <v>0.8</v>
+      </c>
+      <c r="I14">
+        <v>0.8</v>
+      </c>
+      <c r="J14">
         <v>1.2</v>
       </c>
-      <c r="D14">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E14">
-        <v>0.8</v>
-      </c>
-      <c r="F14">
-        <v>0.01</v>
-      </c>
-      <c r="G14">
-        <v>0.9</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>0.9</v>
-      </c>
-      <c r="J14">
-        <v>0.4</v>
-      </c>
       <c r="K14">
         <v>0.01</v>
       </c>
       <c r="L14">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="M14">
         <v>0.4</v>
@@ -1189,310 +1188,310 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15">
+        <v>7.2</v>
+      </c>
+      <c r="C15">
+        <v>7.6</v>
+      </c>
+      <c r="D15">
+        <v>7.4</v>
+      </c>
+      <c r="E15">
+        <v>2.7</v>
+      </c>
+      <c r="F15">
+        <v>0.2</v>
+      </c>
+      <c r="G15">
+        <v>6.6</v>
+      </c>
+      <c r="H15">
+        <v>6.9</v>
+      </c>
+      <c r="I15">
+        <v>6.8</v>
+      </c>
+      <c r="J15">
+        <v>2.1</v>
+      </c>
+      <c r="K15">
+        <v>0.16</v>
+      </c>
+      <c r="L15">
+        <v>0.6</v>
+      </c>
+      <c r="M15">
+        <v>0.6</v>
+      </c>
+      <c r="N15">
+        <v>0.05</v>
+      </c>
+      <c r="O15">
+        <v>0.02</v>
+      </c>
+      <c r="P15">
+        <v>0.03</v>
+      </c>
+      <c r="Q15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C16">
+        <v>1.2</v>
+      </c>
+      <c r="D16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E16">
+        <v>3.3</v>
+      </c>
+      <c r="F16">
+        <v>0.04</v>
+      </c>
+      <c r="G16">
         <v>0.9</v>
       </c>
-      <c r="C15">
+      <c r="H16">
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="I16">
         <v>0.9</v>
       </c>
-      <c r="E15">
-        <v>1.6</v>
-      </c>
-      <c r="F15">
-        <v>0.01</v>
-      </c>
-      <c r="G15">
+      <c r="J16">
+        <v>2.4</v>
+      </c>
+      <c r="K16">
+        <v>0.03</v>
+      </c>
+      <c r="L16">
+        <v>0.2</v>
+      </c>
+      <c r="M16">
+        <v>0.9</v>
+      </c>
+      <c r="N16">
+        <v>0.02</v>
+      </c>
+      <c r="O16">
+        <v>0.01</v>
+      </c>
+      <c r="P16">
+        <v>0.01</v>
+      </c>
+      <c r="Q16">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
         <v>0.8</v>
       </c>
-      <c r="H15">
+      <c r="C17">
+        <v>0.9</v>
+      </c>
+      <c r="D17">
         <v>0.8</v>
       </c>
-      <c r="I15">
+      <c r="E17">
+        <v>2.9</v>
+      </c>
+      <c r="F17">
+        <v>0.02</v>
+      </c>
+      <c r="G17">
+        <v>0.7</v>
+      </c>
+      <c r="H17">
         <v>0.8</v>
       </c>
-      <c r="J15">
-        <v>1.2</v>
-      </c>
-      <c r="K15">
-        <v>0.01</v>
-      </c>
-      <c r="L15">
-        <v>0.1</v>
-      </c>
-      <c r="M15">
-        <v>0.4</v>
-      </c>
-      <c r="N15">
-        <v>0.01</v>
-      </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <v>0.01</v>
-      </c>
-      <c r="Q15">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>30.8</v>
-      </c>
-      <c r="C16">
-        <v>32.4</v>
-      </c>
-      <c r="D16">
-        <v>31.6</v>
-      </c>
-      <c r="E16">
-        <v>2.14</v>
-      </c>
-      <c r="F16">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G16">
-        <v>29.2</v>
-      </c>
-      <c r="H16">
-        <v>30.6</v>
-      </c>
-      <c r="I16">
-        <v>29.9</v>
-      </c>
-      <c r="J16">
-        <v>1.84</v>
-      </c>
-      <c r="K16">
-        <v>0.47</v>
-      </c>
-      <c r="L16">
-        <v>1.7</v>
-      </c>
-      <c r="M16">
-        <v>0.3</v>
-      </c>
-      <c r="N16">
-        <v>0.11</v>
-      </c>
-      <c r="O16">
-        <v>0.03</v>
-      </c>
-      <c r="P16">
-        <v>0.08</v>
-      </c>
-      <c r="Q16">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17">
-        <v>7.2</v>
-      </c>
-      <c r="C17">
-        <v>7.6</v>
-      </c>
-      <c r="D17">
-        <v>7.4</v>
-      </c>
-      <c r="E17">
-        <v>2.7</v>
-      </c>
-      <c r="F17">
-        <v>0.2</v>
-      </c>
-      <c r="G17">
-        <v>6.6</v>
-      </c>
-      <c r="H17">
-        <v>6.9</v>
-      </c>
       <c r="I17">
-        <v>6.8</v>
+        <v>0.7</v>
       </c>
       <c r="J17">
         <v>2.1</v>
       </c>
       <c r="K17">
-        <v>0.16</v>
+        <v>0.02</v>
       </c>
       <c r="L17">
+        <v>0.1</v>
+      </c>
+      <c r="M17">
+        <v>0.8</v>
+      </c>
+      <c r="N17">
+        <v>0.01</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0.01</v>
+      </c>
+      <c r="Q17">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
         <v>0.6</v>
       </c>
-      <c r="M17">
+      <c r="C18">
         <v>0.6</v>
       </c>
-      <c r="N17">
-        <v>0.05</v>
-      </c>
-      <c r="O17">
+      <c r="D18">
+        <v>0.6</v>
+      </c>
+      <c r="E18">
+        <v>1.8</v>
+      </c>
+      <c r="F18">
+        <v>0.01</v>
+      </c>
+      <c r="G18">
+        <v>0.5</v>
+      </c>
+      <c r="H18">
+        <v>0.5</v>
+      </c>
+      <c r="I18">
+        <v>0.5</v>
+      </c>
+      <c r="J18">
+        <v>1.5</v>
+      </c>
+      <c r="K18">
+        <v>0.01</v>
+      </c>
+      <c r="L18">
+        <v>0.1</v>
+      </c>
+      <c r="M18">
+        <v>0.3</v>
+      </c>
+      <c r="N18">
+        <v>0.01</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0.01</v>
+      </c>
+      <c r="Q18">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" collapsed="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C19">
+        <v>4.8</v>
+      </c>
+      <c r="D19">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E19">
+        <v>1.4</v>
+      </c>
+      <c r="F19">
+        <v>0.06</v>
+      </c>
+      <c r="G19">
+        <v>3.8</v>
+      </c>
+      <c r="H19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.04</v>
+      </c>
+      <c r="L19">
+        <v>0.6</v>
+      </c>
+      <c r="M19">
+        <v>0.4</v>
+      </c>
+      <c r="N19">
         <v>0.02</v>
       </c>
-      <c r="P17">
-        <v>0.03</v>
-      </c>
-      <c r="Q17">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C18">
-        <v>1.2</v>
-      </c>
-      <c r="D18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E18">
-        <v>3.3</v>
-      </c>
-      <c r="F18">
-        <v>0.04</v>
-      </c>
-      <c r="G18">
-        <v>0.9</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>0.9</v>
-      </c>
-      <c r="J18">
-        <v>2.4</v>
-      </c>
-      <c r="K18">
-        <v>0.03</v>
-      </c>
-      <c r="L18">
-        <v>0.2</v>
-      </c>
-      <c r="M18">
-        <v>0.9</v>
-      </c>
-      <c r="N18">
+      <c r="O19">
+        <v>0.01</v>
+      </c>
+      <c r="P19">
+        <v>0.01</v>
+      </c>
+      <c r="Q19">
         <v>0.02</v>
       </c>
-      <c r="O18">
-        <v>0.01</v>
-      </c>
-      <c r="P18">
-        <v>0.01</v>
-      </c>
-      <c r="Q18">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19">
-        <v>0.8</v>
-      </c>
-      <c r="C19">
-        <v>0.9</v>
-      </c>
-      <c r="D19">
-        <v>0.8</v>
-      </c>
-      <c r="E19">
-        <v>2.9</v>
-      </c>
-      <c r="F19">
-        <v>0.02</v>
-      </c>
-      <c r="G19">
-        <v>0.7</v>
-      </c>
-      <c r="H19">
-        <v>0.8</v>
-      </c>
-      <c r="I19">
-        <v>0.7</v>
-      </c>
-      <c r="J19">
-        <v>2.1</v>
-      </c>
-      <c r="K19">
-        <v>0.02</v>
-      </c>
-      <c r="L19">
-        <v>0.1</v>
-      </c>
-      <c r="M19">
-        <v>0.8</v>
-      </c>
-      <c r="N19">
-        <v>0.01</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0.01</v>
-      </c>
-      <c r="Q19">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C20">
         <v>0.6</v>
       </c>
       <c r="D20">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="E20">
-        <v>1.8</v>
+        <v>6.1</v>
       </c>
       <c r="F20">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="G20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H20">
         <v>0.5</v>
       </c>
       <c r="I20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J20">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="K20">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="L20">
         <v>0.1</v>
       </c>
       <c r="M20">
-        <v>0.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N20">
         <v>0.01</v>
@@ -1507,215 +1506,109 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21">
-        <v>4.4000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="C21">
-        <v>4.8</v>
+        <v>0.5</v>
       </c>
       <c r="D21">
-        <v>4.5999999999999996</v>
+        <v>0.5</v>
       </c>
       <c r="E21">
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="F21">
-        <v>0.06</v>
+        <v>0.01</v>
       </c>
       <c r="G21">
-        <v>3.8</v>
+        <v>0.4</v>
       </c>
       <c r="H21">
-        <v>4.0999999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="I21">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="K21">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="L21">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="M21">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="N21">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="O21">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="P21">
         <v>0.01</v>
       </c>
       <c r="Q21">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22">
-        <v>0.5</v>
-      </c>
-      <c r="C22">
-        <v>0.6</v>
-      </c>
-      <c r="D22">
-        <v>0.5</v>
-      </c>
-      <c r="E22">
-        <v>6.1</v>
-      </c>
-      <c r="F22">
-        <v>0.03</v>
-      </c>
-      <c r="G22">
-        <v>0.4</v>
-      </c>
-      <c r="H22">
-        <v>0.5</v>
-      </c>
-      <c r="I22">
-        <v>0.4</v>
-      </c>
-      <c r="J22">
-        <v>5</v>
-      </c>
-      <c r="K22">
-        <v>0.02</v>
-      </c>
-      <c r="L22">
-        <v>0.1</v>
-      </c>
-      <c r="M22">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="N22">
-        <v>0.01</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>0.01</v>
-      </c>
-      <c r="Q22">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23">
-        <v>0.4</v>
+        <v>100</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>100</v>
       </c>
       <c r="D23">
-        <v>0.5</v>
+        <v>100</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>3.21</v>
       </c>
       <c r="F23">
-        <v>0.01</v>
+        <v>3.18</v>
       </c>
       <c r="G23">
-        <v>0.4</v>
+        <v>100</v>
       </c>
       <c r="H23">
-        <v>0.4</v>
+        <v>100</v>
       </c>
       <c r="I23">
-        <v>0.4</v>
+        <v>100</v>
       </c>
       <c r="J23">
-        <v>1.3</v>
+        <v>2.98</v>
       </c>
       <c r="K23">
-        <v>0.01</v>
+        <v>0.23</v>
       </c>
       <c r="L23">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M23">
-        <v>0.7</v>
+        <v>0.23</v>
       </c>
       <c r="N23">
-        <v>0.01</v>
+        <v>0.23</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="P23">
-        <v>0.01</v>
+        <v>0.19</v>
       </c>
       <c r="Q23">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25">
-        <v>100</v>
-      </c>
-      <c r="C25">
-        <v>100</v>
-      </c>
-      <c r="D25">
-        <v>100</v>
-      </c>
-      <c r="E25">
-        <v>3.21</v>
-      </c>
-      <c r="F25">
-        <v>3.18</v>
-      </c>
-      <c r="G25">
-        <v>100</v>
-      </c>
-      <c r="H25">
-        <v>100</v>
-      </c>
-      <c r="I25">
-        <v>100</v>
-      </c>
-      <c r="J25">
-        <v>2.98</v>
-      </c>
-      <c r="K25">
-        <v>0.23</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0.23</v>
-      </c>
-      <c r="N25">
-        <v>0.23</v>
-      </c>
-      <c r="O25">
-        <v>0.04</v>
-      </c>
-      <c r="P25">
-        <v>0.19</v>
-      </c>
-      <c r="Q25">
         <v>0.23</v>
       </c>
     </row>
@@ -1731,7 +1624,9 @@
   </sheetPr>
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1764,7 +1659,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1810,7 +1705,7 @@
         <v>18</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>20</v>
@@ -1822,9 +1717,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>27.6</v>
@@ -1866,9 +1761,9 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="9" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>16.8</v>
@@ -1910,9 +1805,9 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>7.2</v>
@@ -1954,9 +1849,9 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>1.1000000000000001</v>
@@ -1998,9 +1893,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>0.6</v>
@@ -2042,9 +1937,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>10.8</v>
@@ -2086,9 +1981,9 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="14" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>5.2</v>
@@ -2130,9 +2025,9 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="15" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>1.4</v>
@@ -2174,9 +2069,9 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>12.9</v>
@@ -2218,9 +2113,9 @@
         <v>-0.19</v>
       </c>
     </row>
-    <row r="17" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>6.7</v>
@@ -2262,9 +2157,9 @@
         <v>-0.12</v>
       </c>
     </row>
-    <row r="18" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>1.3</v>
@@ -2306,9 +2201,9 @@
         <v>-0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>0.8</v>
@@ -2350,9 +2245,9 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>0.7</v>
@@ -2394,9 +2289,9 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:14" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>3.4</v>
@@ -2438,9 +2333,9 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>0.9</v>
@@ -2482,9 +2377,9 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:14" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>0.7</v>
@@ -2528,7 +2423,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -2579,7 +2474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26097E21-1CB5-7248-8225-6FC82F722EB1}">
   <dimension ref="A6:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2592,32 +2487,32 @@
   <sheetData>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6">
         <v>6.25</v>
@@ -2626,15 +2521,15 @@
         <v>1.23E-2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C11" s="6">
         <v>5.8</v>
@@ -2643,15 +2538,15 @@
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C12" s="6">
         <v>4.0999999999999996</v>
@@ -2660,15 +2555,15 @@
         <v>9.4999999999999998E-3</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="C13" s="6">
         <v>3.5</v>
@@ -2677,15 +2572,15 @@
         <v>6.1999999999999998E-3</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="C14" s="6">
         <v>2.2000000000000002</v>
@@ -2694,15 +2589,15 @@
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="C15" s="6">
         <v>1.9</v>
@@ -2711,15 +2606,15 @@
         <v>-3.8E-3</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="C16" s="6">
         <v>2.1</v>
@@ -2728,15 +2623,15 @@
         <v>-2.3999999999999998E-3</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C17" s="6">
         <v>1.75</v>
@@ -2745,15 +2640,15 @@
         <v>-1.9E-3</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C18" s="6">
         <v>1.1000000000000001</v>
@@ -2762,15 +2657,15 @@
         <v>-1.1999999999999999E-3</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="C19" s="6">
         <v>0.95</v>
@@ -2779,15 +2674,15 @@
         <v>-8.9999999999999998E-4</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="C20" s="6">
         <v>0.5</v>
@@ -2796,15 +2691,15 @@
         <v>1E-4</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="C21" s="6">
         <v>0</v>
@@ -2813,7 +2708,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>